<commit_message>
TEST GROUP DATA CLEANING AND EDA
</commit_message>
<xml_diff>
--- a/working_data/control_group.xlsx
+++ b/working_data/control_group.xlsx
@@ -683,6 +683,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="control_group" displayName="control_group" ref="A1:J31" totalsRowShown="0">
+  <autoFilter ref="A1:J31"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Campaign Name"/>
+    <tableColumn id="2" name="Date"/>
+    <tableColumn id="3" name="Spend [USD]"/>
+    <tableColumn id="4" name="# of Impressions"/>
+    <tableColumn id="5" name="Reach"/>
+    <tableColumn id="6" name="# of Website Clicks"/>
+    <tableColumn id="7" name="# of Searches"/>
+    <tableColumn id="8" name="# of View Content"/>
+    <tableColumn id="9" name="# of Add to Cart"/>
+    <tableColumn id="10" name="# of Purchase"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -951,21 +970,21 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1941,5 +1960,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>